<commit_message>
scraped data from 1990 to 2020
</commit_message>
<xml_diff>
--- a/kladd.xlsx
+++ b/kladd.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Truls\Documents\git\new_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{504E9FE2-6F1E-4DF2-A1E6-AC5C08859879}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A8B4E6B-9E8B-46A0-9DAF-AB784A929837}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F8AB8032-EF32-437F-B496-18F732A2BFEE}"/>
+    <workbookView xWindow="28680" yWindow="-5520" windowWidth="38640" windowHeight="21240" xr2:uid="{F8AB8032-EF32-437F-B496-18F732A2BFEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -104,9 +104,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="168" formatCode="0.0\ %"/>
-    <numFmt numFmtId="170" formatCode="0.000"/>
-    <numFmt numFmtId="171" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0\ %"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -151,11 +151,11 @@
       <alignment textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7BFB37C-E636-4237-9688-B57C5790C27E}">
-  <dimension ref="A1:Y3"/>
+  <dimension ref="A1:Y4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y3" sqref="Y3"/>
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,7 +600,7 @@
         <v>20</v>
       </c>
       <c r="P2" s="4">
-        <f>(H2-J2)*O2*IF((C2-D2)&lt;2,1,IF((C2-D2)=2,1.5,IF((C2-D2)=3,1.75,1+3/4+((C2-D2)-3)/8)))</f>
+        <f>(H2-J2)*O2*L2</f>
         <v>1.8735892364187923</v>
       </c>
       <c r="Q2" s="5">
@@ -683,7 +683,7 @@
         <v>20</v>
       </c>
       <c r="P3" s="4">
-        <f>(H3-J3)*O3*IF((C3-D3)&lt;2,1,IF((C3-D3)=2,1.5,IF((C3-D3)=3,1.75,1+3/4+((C3-D3)-3)/8)))</f>
+        <f>(H3-J3)*O3*L3</f>
         <v>5.2072149128608718</v>
       </c>
       <c r="Q3" s="5">
@@ -715,6 +715,89 @@
       <c r="Y3" s="2">
         <f>IF(E3=Q3,0,IF(V3=E3,100,"error"))</f>
         <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>1600</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1600</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2">
+        <f>IF(C4&gt;D4,1,IF(D4&gt;C4,0,0.5))</f>
+        <v>0.5</v>
+      </c>
+      <c r="I4" s="2">
+        <f>IF(C4&gt;D4,0,IF(D4&gt;C4,1,0.5))</f>
+        <v>0.5</v>
+      </c>
+      <c r="J4" s="3">
+        <f>1/(1+10^((-A4+B4)/400))</f>
+        <v>0.5</v>
+      </c>
+      <c r="K4" s="3">
+        <f>1/(1+10^((-A4+B4-100)/400))</f>
+        <v>0.64006499980288512</v>
+      </c>
+      <c r="L4" s="7">
+        <f>IF((C4-D4)&lt;2,1,IF((C4-D4)=2,1.5,IF((C4-D4)=3,1.75,1+3/4+((C4-D4)-3)/8)))</f>
+        <v>1</v>
+      </c>
+      <c r="M4" s="7"/>
+      <c r="N4" s="6" t="e">
+        <f>E4/L4/(H4-J4)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O4" s="2" t="e">
+        <f>ROUND(N4/10,0)*10</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P4" s="4" t="e">
+        <f>(H4-J4)*O4*L4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q4" s="5" t="e">
+        <f>ROUND(P4,0)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R4" s="5"/>
+      <c r="S4" s="4">
+        <f>E4/L4/(H4-K4)</f>
+        <v>0</v>
+      </c>
+      <c r="T4" s="2">
+        <f>ROUND(S4/10,0)*10</f>
+        <v>0</v>
+      </c>
+      <c r="U4" s="4">
+        <f>(H4-K4)*T4*IF((C4-D4)&lt;2,1,IF((C4-D4)=2,1.5,IF((C4-D4)=3,1.75,1+3/4+((C4-D4)-3)/8)))</f>
+        <v>0</v>
+      </c>
+      <c r="V4" s="5">
+        <f>ROUND(U4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="W4" s="5"/>
+      <c r="X4" s="2" t="e">
+        <f>IF(E4=Q4,O4,IF(V4=E4,T4,"error"))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y4" s="2" t="e">
+        <f>IF(E4=Q4,0,IF(V4=E4,100,"error"))</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>